<commit_message>
Read data from excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testcases/Testcases.xlsx
+++ b/src/main/resources/testcases/Testcases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\seleniumwithjava\src\main\resources\automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\seleniumwithjava\src\main\resources\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB1A2B0-DC0B-4DE6-A71A-7A996CBB1661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A6C955-23B7-4A14-A459-41FF5C97AF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Web Application</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -65,6 +62,25 @@
     <t>1.Go to https://www.covid19india.org/
 2.Get all states's Confirmed, Active, Recovered, Deceased count
 3.Print all the count in excel sheet</t>
+  </si>
+  <si>
+    <t>Data driven testing</t>
+  </si>
+  <si>
+    <t>Web Application/Topic</t>
+  </si>
+  <si>
+    <t>Read data from excel sheet</t>
+  </si>
+  <si>
+    <t>Write data in excel sheet</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Read the values from website and put into the lists.
+Need to write into the excel sheet.</t>
   </si>
 </sst>
 </file>
@@ -388,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,52 +416,80 @@
     <col min="2" max="2" width="47.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.21875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D20" xr:uid="{0B3C860B-8272-4D57-BFAE-CE2879CEF5A8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D3:D19" xr:uid="{0B3C860B-8272-4D57-BFAE-CE2879CEF5A8}">
       <formula1>"Done,In-Progress"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>